<commit_message>
Updates: DPP Updates 19/02/2015
</commit_message>
<xml_diff>
--- a/files/procurement_plan_WORKS.xlsx
+++ b/files/procurement_plan_WORKS.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>Annex - III (b)</t>
   </si>
@@ -29,25 +29,25 @@
     <t xml:space="preserve">Project Name: </t>
   </si>
   <si>
-    <t>Aid Effectiveness Project for ERD</t>
+    <t>Rehabilitation/Renovation of Electrical and Arboriculture Work of Planning Commission campus at sher-e-Bangla Nagar, Dhaka.</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry/Division: </t>
   </si>
   <si>
-    <t xml:space="preserve">Ministry of Agriculture
+    <t xml:space="preserve">Ministry of Planning, Planning Division
 </t>
   </si>
   <si>
     <t xml:space="preserve">Agency: </t>
   </si>
   <si>
-    <t xml:space="preserve"> Bangladesh Institute of Administration &amp; Management Foundation (BIAM)
-Bangladesh Institute of Nuclear Agriculture (BINA)
+    <t xml:space="preserve">Planning Division
+Public Works Department (PWD)
 </t>
   </si>
   <si>
-    <t>Total GoB (FE): 19.03(21.43)</t>
+    <t>Total GoB (FE): 703.1600000000001(0)</t>
   </si>
   <si>
     <t xml:space="preserve">Procuring Entity Name and Code: </t>
@@ -56,7 +56,7 @@
     <t>Procuring Entity</t>
   </si>
   <si>
-    <t>Total PA (RPA): 37(29)</t>
+    <t>Total PA (RPA): 0(0)</t>
   </si>
   <si>
     <t xml:space="preserve">Project/Programme Code: </t>
@@ -65,7 +65,7 @@
     <t>Project/Programme Code</t>
   </si>
   <si>
-    <t>Others (FE): 11.77(11.75)</t>
+    <t>Others (FE): 0(0)</t>
   </si>
   <si>
     <t>Package No.</t>
@@ -106,46 +106,119 @@
     <t>Completion of Contract</t>
   </si>
   <si>
-    <t>xxxx</t>
-  </si>
-  <si>
-    <t>sdfas</t>
-  </si>
-  <si>
-    <t>TSTM(INT)</t>
-  </si>
-  <si>
-    <t>2014-10-08</t>
-  </si>
-  <si>
-    <t>2014-10-21</t>
-  </si>
-  <si>
-    <t>asdfa</t>
-  </si>
-  <si>
-    <t>RFQM(NCT)</t>
-  </si>
-  <si>
-    <t>2014-10-15</t>
-  </si>
-  <si>
-    <t>adsadf</t>
-  </si>
-  <si>
-    <t>sdf</t>
-  </si>
-  <si>
-    <t>DPM(NCT)</t>
-  </si>
-  <si>
-    <t>GoB</t>
-  </si>
-  <si>
-    <t>UNDP</t>
-  </si>
-  <si>
-    <t>2014-10-22</t>
+    <t>1-wd</t>
+  </si>
+  <si>
+    <t>Supply and Replacement of damaged underground main cable of NEC building and Necessary work.</t>
+  </si>
+  <si>
+    <t>OTM(NCT)</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>GOB</t>
+  </si>
+  <si>
+    <t>0000-00-00</t>
+  </si>
+  <si>
+    <t>2015-04-09</t>
+  </si>
+  <si>
+    <t>2015-06-10</t>
+  </si>
+  <si>
+    <t>2015-12-30</t>
+  </si>
+  <si>
+    <t>2-wd</t>
+  </si>
+  <si>
+    <t>Supply and Replacement of damaged Service cable of Building No 3,4,5 &amp; 6</t>
+  </si>
+  <si>
+    <t>3-wd</t>
+  </si>
+  <si>
+    <t>Supply and Replacement of damaged air cooler of different capacities in planning Division</t>
+  </si>
+  <si>
+    <t>4-wd</t>
+  </si>
+  <si>
+    <t>Supply and Replacement of damaged HT Switch gear, LT switch Gear, PFI and necessary works of 400KVA Sub-Station.</t>
+  </si>
+  <si>
+    <t>5-wd</t>
+  </si>
+  <si>
+    <t>Supply and Replacement of damaged Duct pump motor set of 90 Ton central A/C and necessary work</t>
+  </si>
+  <si>
+    <t>6-wd</t>
+  </si>
+  <si>
+    <t>Supply and Replacement of damaged sub main power line, control switch SPDB and necessary work of building No-l-18(GF to 2nd F) of planning Commission complex.</t>
+  </si>
+  <si>
+    <t>7-wd</t>
+  </si>
+  <si>
+    <t>Supply and Replacement of Oil in X-former, different panel board and other necessary works.</t>
+  </si>
+  <si>
+    <t>8-wd</t>
+  </si>
+  <si>
+    <t>Supply and Replacement of Metal halide light and necessary works</t>
+  </si>
+  <si>
+    <t>9-wd</t>
+  </si>
+  <si>
+    <t>Supply and Replacement of 2000KVA Sub-Station in lieu of 800 KVA sub-Station and other necessary works</t>
+  </si>
+  <si>
+    <t>10-wd</t>
+  </si>
+  <si>
+    <t>Supply and Installation of L.C work of different building in planning
+commission campus</t>
+  </si>
+  <si>
+    <t>11-wd</t>
+  </si>
+  <si>
+    <t>Supply and Installation of Security light and necessary work in planning Commission campus.</t>
+  </si>
+  <si>
+    <t>12-wd</t>
+  </si>
+  <si>
+    <t>Supply and Installation of damaged main service cable and necessary work west side Building No 3,4,5,6,11,12 of planning Commission campus.</t>
+  </si>
+  <si>
+    <t>13-wd</t>
+  </si>
+  <si>
+    <t>Supply and Installation of damaged main service cable and necessary (work of East side Building No 1,2,7,8,9,10,15,16 of planning Commission</t>
+  </si>
+  <si>
+    <t>14-wd</t>
+  </si>
+  <si>
+    <t>Arboriculture work of planning commission Campus</t>
+  </si>
+  <si>
+    <t>2016-03-20</t>
+  </si>
+  <si>
+    <t>15-wd</t>
+  </si>
+  <si>
+    <t>Supply and Installation of CCTV camera in Planning commission Supply and Installation of CCTV camera in Planning commission</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -597,7 +670,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1"/>
   </sheetViews>
@@ -813,122 +886,586 @@
         <v>29</v>
       </c>
       <c r="C14" s="9">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="D14" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="F14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="H14" s="13">
+        <v>80.12</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="13">
+        <v>8.88</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="9">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="13">
+        <v>98.19</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="13">
+        <v>16.64</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="13">
+        <v>25.31</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="13">
+        <v>68.93</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="13">
+        <v>15.59</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="13">
+        <v>12.89</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="13">
+        <v>103.33</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="13">
+        <v>44.58</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="B24" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="H24" s="13">
+        <v>19.15</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L14" s="9" t="s">
+      <c r="H25" s="13">
+        <v>59.38</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="9">
-        <v>4</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="H26" s="13">
+        <v>64.21</v>
+      </c>
+      <c r="I26" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="9">
-        <v>4</v>
-      </c>
-      <c r="D15" s="9">
-        <v>1</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="J26" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="13">
-        <v>5</v>
-      </c>
-      <c r="I15" s="9" t="s">
+      <c r="K26" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="L26" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="H27" s="13">
+        <v>38</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="L15" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="9">
-        <v>43</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="9">
-        <v>12</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="13">
-        <v>12</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="16">
-        <f>SUM(H7:H16)</f>
-        <v>72</v>
-      </c>
-      <c r="I17" s="15" t="s"/>
-      <c r="J17" s="15" t="s"/>
-      <c r="K17" s="15" t="s"/>
-      <c r="L17" s="15" t="s"/>
+      <c r="H28" s="13">
+        <v>39.76</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16">
+        <f>SUM(H7:H28)</f>
+        <v>694.96</v>
+      </c>
+      <c r="I29" s="15" t="s"/>
+      <c r="J29" s="15" t="s"/>
+      <c r="K29" s="15" t="s"/>
+      <c r="L29" s="15" t="s"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -948,7 +1485,7 @@
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="J10:L10"/>
-    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A29:G29"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>